<commit_message>
Updated code to match the last changes, Fixed issue with 'added VIN' that became invalid in the system, added test in scorpions suite, made small refactoring
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/uploadAddedVIN_CA_CHOICE_.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/uploadAddedVIN_CA_CHOICE_.xlsx
@@ -155,9 +155,6 @@
     <t>SYMBOL_2000_CHOICE_T</t>
   </si>
   <si>
-    <t>BBBKN3DD&amp;E</t>
-  </si>
-  <si>
     <t>BI_SYMBOL</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>TEST</t>
+  </si>
+  <si>
+    <t>1FDEU15H&amp;K</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:AJ3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,33 +644,33 @@
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>42</v>
@@ -697,13 +697,13 @@
         <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>29</v>
@@ -754,16 +754,16 @@
         <v>38</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AG2">
         <v>20000101</v>
@@ -775,7 +775,7 @@
         <v>38</v>
       </c>
       <c r="AJ2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.3">

</xml_diff>